<commit_message>
Adds the concept of a group, which is basically a bunch of lines surrounded by empty line.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Worksheet.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\excel\poi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216F4256-13CA-4093-980E-4E8299D4B3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B55E1D1-7327-4931-B7D7-B597CC322C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28830" yWindow="5145" windowWidth="15660" windowHeight="11145" firstSheet="13" activeTab="13" xr2:uid="{2B1CA52D-E10F-49D8-8A0A-7B3A987640D9}"/>
+    <workbookView xWindow="28800" yWindow="6180" windowWidth="15660" windowHeight="11145" firstSheet="28" activeTab="29" xr2:uid="{2B1CA52D-E10F-49D8-8A0A-7B3A987640D9}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidTinyWorksheet" sheetId="25" r:id="rId1"/>
@@ -41,7 +41,9 @@
     <sheet name="BooleanInHeader" sheetId="9" r:id="rId26"/>
     <sheet name="DateInHeader" sheetId="10" r:id="rId27"/>
     <sheet name="NumericFormulaInHeader" sheetId="11" r:id="rId28"/>
-    <sheet name="Notas de Corretagem" sheetId="3" r:id="rId29"/>
+    <sheet name="GroupsNoEmptyLineAfterHeader" sheetId="3" r:id="rId29"/>
+    <sheet name="GroupsEmptyLineAfterHeader" sheetId="45" r:id="rId30"/>
+    <sheet name="Notas de Corretagem (2)" sheetId="44" r:id="rId31"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -70,7 +72,7 @@
     <author>Andrei Diego Cardoso</author>
   </authors>
   <commentList>
-    <comment ref="K47" authorId="0" shapeId="0" xr:uid="{D27EA324-0D44-4ECA-8D25-001F24643458}">
+    <comment ref="K47" authorId="0" shapeId="0" xr:uid="{EC909B4E-D782-4721-AFF2-7310C40A2E4B}">
       <text>
         <r>
           <rPr>
@@ -94,7 +96,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K48" authorId="0" shapeId="0" xr:uid="{DD76F6EF-E3E1-4F2D-8812-0F27CD659C41}">
+    <comment ref="K48" authorId="0" shapeId="0" xr:uid="{ADCE1A0C-FF2B-4E22-8B38-A3925811EF28}">
       <text>
         <r>
           <rPr>
@@ -118,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K51" authorId="0" shapeId="0" xr:uid="{C98B32A7-6A74-4A4A-9741-638FF540D7A0}">
+    <comment ref="K51" authorId="0" shapeId="0" xr:uid="{85A7F20B-54CE-4213-BDF6-D58F17A14214}">
       <text>
         <r>
           <rPr>
@@ -142,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K59" authorId="0" shapeId="0" xr:uid="{5116CEC1-7D29-4143-A8B1-C43DF45A7866}">
+    <comment ref="K59" authorId="0" shapeId="0" xr:uid="{A6C02BFB-F8A8-4C66-B4DB-DB3FBEA97D31}">
       <text>
         <r>
           <rPr>
@@ -166,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K61" authorId="0" shapeId="0" xr:uid="{05F18A6F-D06C-4410-B4BE-74FBF521DF30}">
+    <comment ref="K61" authorId="0" shapeId="0" xr:uid="{C2222EC9-A9AF-47E6-AAB8-B3F1DDCC717C}">
       <text>
         <r>
           <rPr>
@@ -190,7 +192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L100" authorId="0" shapeId="0" xr:uid="{C52CB742-45DE-4716-A2E3-FE4A4B034696}">
+    <comment ref="L100" authorId="0" shapeId="0" xr:uid="{4C17B194-5D43-4C82-A407-DC4839763B10}">
       <text>
         <r>
           <rPr>
@@ -214,7 +216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A112" authorId="1" shapeId="0" xr:uid="{8BC4BBC6-66AE-4E53-A85E-46BBDEB42129}">
+    <comment ref="A112" authorId="1" shapeId="0" xr:uid="{2633D12F-1F8E-4C55-A0BE-758F2FEA8644}">
       <text>
         <r>
           <rPr>
@@ -227,7 +229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H112" authorId="0" shapeId="0" xr:uid="{00980C28-CB01-401C-B8E1-67A147D40CDE}">
+    <comment ref="H112" authorId="0" shapeId="0" xr:uid="{B980EECC-067C-45D0-9143-570E446FA9AD}">
       <text>
         <r>
           <rPr>
@@ -251,7 +253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K112" authorId="0" shapeId="0" xr:uid="{D8B5AB84-3803-4580-B971-4ADF0CA35058}">
+    <comment ref="K112" authorId="0" shapeId="0" xr:uid="{5756160B-26E5-41CB-AAFA-253EABFED42E}">
       <text>
         <r>
           <rPr>
@@ -275,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A114" authorId="1" shapeId="0" xr:uid="{0BED7DE9-A29D-4AC4-B826-916723B5AEF5}">
+    <comment ref="A114" authorId="1" shapeId="0" xr:uid="{015EEE74-DD5C-4B26-B70E-F9EA1AF20857}">
       <text>
         <r>
           <rPr>
@@ -288,7 +290,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H114" authorId="0" shapeId="0" xr:uid="{452E0819-BFAE-4026-8491-FB6E1EE35A84}">
+    <comment ref="H114" authorId="0" shapeId="0" xr:uid="{CA7293AF-F202-4359-8FFF-04A4DF2ACE96}">
       <text>
         <r>
           <rPr>
@@ -312,7 +314,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K114" authorId="0" shapeId="0" xr:uid="{D6E1E588-EC18-4252-8FC1-86DCEBA05147}">
+    <comment ref="K114" authorId="0" shapeId="0" xr:uid="{F9CA2874-7AFB-46F8-B8DE-6CCAD99A4C3E}">
       <text>
         <r>
           <rPr>
@@ -336,7 +338,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A118" authorId="1" shapeId="0" xr:uid="{AC636639-6F7C-4ED2-9E5A-3F6245094D0F}">
+    <comment ref="A118" authorId="1" shapeId="0" xr:uid="{1C0F4A09-E623-4DE0-AAA5-00398ED854D4}">
       <text>
         <r>
           <rPr>
@@ -349,7 +351,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H118" authorId="0" shapeId="0" xr:uid="{F12EDCEF-EB58-42FE-B492-0D848118D272}">
+    <comment ref="H118" authorId="0" shapeId="0" xr:uid="{18329E89-53A4-477B-A7EB-C2E124ED0E12}">
       <text>
         <r>
           <rPr>
@@ -373,7 +375,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K118" authorId="0" shapeId="0" xr:uid="{FE94D7AB-BA1E-492A-8046-2516CA1287D9}">
+    <comment ref="K118" authorId="0" shapeId="0" xr:uid="{F8EB032D-C81E-402E-8C17-EC410A7D3674}">
       <text>
         <r>
           <rPr>
@@ -397,7 +399,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K122" authorId="0" shapeId="0" xr:uid="{87DAA65E-EFBC-4DB9-98D5-CED1EC873E70}">
+    <comment ref="K122" authorId="0" shapeId="0" xr:uid="{A730B32F-B34D-4CB2-86BC-61D6F7290E27}">
       <text>
         <r>
           <rPr>
@@ -421,7 +423,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A126" authorId="1" shapeId="0" xr:uid="{8691C67D-D253-4009-8822-FBE56B87D326}">
+    <comment ref="A126" authorId="1" shapeId="0" xr:uid="{5B40F890-522E-4E67-B449-73677B80BC5A}">
       <text>
         <r>
           <rPr>
@@ -434,7 +436,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H126" authorId="0" shapeId="0" xr:uid="{36ABECE1-4DF2-4604-B56F-E630F75BC7AE}">
+    <comment ref="H126" authorId="0" shapeId="0" xr:uid="{6D3F460A-F4F2-40EF-8718-88F2965BE22D}">
       <text>
         <r>
           <rPr>
@@ -458,7 +460,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A127" authorId="1" shapeId="0" xr:uid="{B6756495-24F2-471F-9D14-04F03A4A4F1F}">
+    <comment ref="A127" authorId="1" shapeId="0" xr:uid="{D24FC818-1BFB-44CC-BAF4-7549EB4B4AC6}">
       <text>
         <r>
           <rPr>
@@ -471,7 +473,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H127" authorId="0" shapeId="0" xr:uid="{FA5966D0-D1ED-415A-B775-A114E68AD764}">
+    <comment ref="H127" authorId="0" shapeId="0" xr:uid="{D15D0806-E04D-4C50-8769-489BFF27C551}">
       <text>
         <r>
           <rPr>
@@ -495,7 +497,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A130" authorId="1" shapeId="0" xr:uid="{FF5C3581-2CCD-4AA4-9789-6A3DAB2AFC49}">
+    <comment ref="A130" authorId="1" shapeId="0" xr:uid="{E5087F0B-EC1B-42F5-B879-5B197BA2FA56}">
       <text>
         <r>
           <rPr>
@@ -508,7 +510,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H130" authorId="0" shapeId="0" xr:uid="{3BDDA99E-90FF-43A5-9DF5-4C9F565D4D8A}">
+    <comment ref="H130" authorId="0" shapeId="0" xr:uid="{79DC711F-B3FF-4267-B585-1A979090AAC1}">
       <text>
         <r>
           <rPr>
@@ -532,7 +534,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A131" authorId="1" shapeId="0" xr:uid="{85C19A47-0395-42E5-A08E-EFB531F97361}">
+    <comment ref="A131" authorId="1" shapeId="0" xr:uid="{C6350277-B836-47E1-A012-7164A4DC396E}">
       <text>
         <r>
           <rPr>
@@ -545,7 +547,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H131" authorId="0" shapeId="0" xr:uid="{3FDA379C-8958-4EC6-AAC8-8BD3DAE24F69}">
+    <comment ref="H131" authorId="0" shapeId="0" xr:uid="{81485AA1-1780-4B9B-988E-94F438486790}">
       <text>
         <r>
           <rPr>
@@ -569,7 +571,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A134" authorId="1" shapeId="0" xr:uid="{FE9E1B59-ADC9-42D7-A95A-EA94C150E0B2}">
+    <comment ref="A134" authorId="1" shapeId="0" xr:uid="{6B863261-8744-4728-A50F-3EE2ECFAEE19}">
       <text>
         <r>
           <rPr>
@@ -582,7 +584,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H134" authorId="0" shapeId="0" xr:uid="{456D3B9D-5C64-4008-B2CF-CA4BE4943C58}">
+    <comment ref="H134" authorId="0" shapeId="0" xr:uid="{EE4FE3B1-236E-41A6-9C40-8578B0F321CB}">
       <text>
         <r>
           <rPr>
@@ -606,7 +608,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A136" authorId="1" shapeId="0" xr:uid="{57316440-BB4E-47E4-A139-A58D96AAB454}">
+    <comment ref="A136" authorId="1" shapeId="0" xr:uid="{A3A8988B-847A-413E-BD70-6032F9F1FA7F}">
       <text>
         <r>
           <rPr>
@@ -619,7 +621,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H136" authorId="0" shapeId="0" xr:uid="{C0D6BFBD-D740-4859-AC3B-2A7EF790DFDB}">
+    <comment ref="H136" authorId="0" shapeId="0" xr:uid="{97E777B1-959C-4526-B587-63AF8F008B12}">
       <text>
         <r>
           <rPr>
@@ -643,7 +645,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A138" authorId="1" shapeId="0" xr:uid="{78982DFA-F177-4888-8829-3BED2371E993}">
+    <comment ref="A138" authorId="1" shapeId="0" xr:uid="{F15CE9B1-BDFF-4ABF-9608-F20E2C08F530}">
       <text>
         <r>
           <rPr>
@@ -656,7 +658,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H138" authorId="0" shapeId="0" xr:uid="{B6B3F90D-F403-44A9-82A6-CBBA4038BE9F}">
+    <comment ref="H138" authorId="0" shapeId="0" xr:uid="{899A30CF-E892-4651-8243-069088D0C3BB}">
       <text>
         <r>
           <rPr>
@@ -680,7 +682,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A140" authorId="1" shapeId="0" xr:uid="{B2ED06E0-1A0F-40DE-A9A6-FC9804A8D93C}">
+    <comment ref="A140" authorId="1" shapeId="0" xr:uid="{0E9EC922-E9B8-4D8C-A2BA-B0C4923988B6}">
       <text>
         <r>
           <rPr>
@@ -694,7 +696,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H140" authorId="0" shapeId="0" xr:uid="{2888ACB4-FF81-41E6-9945-CC2F98A5DB65}">
+    <comment ref="H140" authorId="0" shapeId="0" xr:uid="{2EF9655E-DC45-4F5F-9082-32FE4224E7F5}">
       <text>
         <r>
           <rPr>
@@ -718,7 +720,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I146" authorId="0" shapeId="0" xr:uid="{2517E4B6-3DF7-44F8-AD7E-64021F08ADEF}">
+    <comment ref="I146" authorId="0" shapeId="0" xr:uid="{4B5A2E9E-44B0-4FF2-AF1C-20763178970E}">
       <text>
         <r>
           <rPr>
@@ -742,7 +744,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H160" authorId="0" shapeId="0" xr:uid="{8F9595E3-3A7D-41BA-8995-5AFAA82957A0}">
+    <comment ref="H160" authorId="0" shapeId="0" xr:uid="{AD303ABF-921D-4D61-9D30-C06141BDD0ED}">
       <text>
         <r>
           <rPr>
@@ -766,7 +768,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H162" authorId="0" shapeId="0" xr:uid="{40EAB5B6-827B-4AD4-BA52-1AA1F2F1F6FD}">
+    <comment ref="H162" authorId="0" shapeId="0" xr:uid="{79326FA8-CA18-43B8-A4BB-8407C7CAD033}">
       <text>
         <r>
           <rPr>
@@ -790,7 +792,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H165" authorId="0" shapeId="0" xr:uid="{F5043DEB-240D-4AC8-AB67-0387562322D7}">
+    <comment ref="H165" authorId="0" shapeId="0" xr:uid="{BB10696F-7AAB-4751-A244-C1160A2B6501}">
       <text>
         <r>
           <rPr>
@@ -814,7 +816,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A167" authorId="0" shapeId="0" xr:uid="{A359B85D-F892-4E7F-89E8-229FF633E14D}">
+    <comment ref="A167" authorId="0" shapeId="0" xr:uid="{8A1EA0EB-2FA7-44B4-8BD7-5341F0520BA2}">
       <text>
         <r>
           <rPr>
@@ -838,7 +840,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A169" authorId="0" shapeId="0" xr:uid="{5EF3E748-5D9B-4B07-817D-57AAFDF6C6FF}">
+    <comment ref="A169" authorId="0" shapeId="0" xr:uid="{D9BF6C9B-0597-40F6-BE13-D5AD293B7F14}">
       <text>
         <r>
           <rPr>
@@ -862,7 +864,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A170" authorId="0" shapeId="0" xr:uid="{A3C3CEBB-555A-4C30-A644-88745F6EC5C1}">
+    <comment ref="A170" authorId="0" shapeId="0" xr:uid="{A208E636-C097-4865-83FF-8A2A333C8D35}">
       <text>
         <r>
           <rPr>
@@ -886,7 +888,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A171" authorId="0" shapeId="0" xr:uid="{B7542974-B640-49C4-9E04-A4006403E3FA}">
+    <comment ref="A171" authorId="0" shapeId="0" xr:uid="{D960D0E0-DCF3-4B90-9FAD-1F7E0365D61E}">
       <text>
         <r>
           <rPr>
@@ -910,7 +912,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A172" authorId="0" shapeId="0" xr:uid="{A2F0B55C-0F4C-4CB6-BDB4-ED6B0A173FFE}">
+    <comment ref="A172" authorId="0" shapeId="0" xr:uid="{522A888B-999E-406D-B63B-CE3E33095141}">
       <text>
         <r>
           <rPr>
@@ -934,7 +936,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A173" authorId="0" shapeId="0" xr:uid="{01D5F7D7-0C85-4285-937D-3F9D19C3D414}">
+    <comment ref="A173" authorId="0" shapeId="0" xr:uid="{D9FAC5E5-E2FD-44D5-B318-E97DDF1DB657}">
       <text>
         <r>
           <rPr>
@@ -958,7 +960,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A174" authorId="0" shapeId="0" xr:uid="{AAA985AB-F4FC-4CC8-ABFC-69DD8EDBB27B}">
+    <comment ref="A174" authorId="0" shapeId="0" xr:uid="{15F0D375-B74F-4E90-9045-5D3B3C0EAB4D}">
       <text>
         <r>
           <rPr>
@@ -982,7 +984,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A175" authorId="0" shapeId="0" xr:uid="{06D480EE-C211-438B-BEF3-69AFCDDF6F8E}">
+    <comment ref="A175" authorId="0" shapeId="0" xr:uid="{C5A7056C-BC5E-4FC6-A87E-2AB2204DA73F}">
       <text>
         <r>
           <rPr>
@@ -1006,7 +1008,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A176" authorId="0" shapeId="0" xr:uid="{BC010A21-6358-426A-9639-88C9EB49F4E8}">
+    <comment ref="A176" authorId="0" shapeId="0" xr:uid="{AD51325A-E860-422A-9D9B-46977C1A33CB}">
       <text>
         <r>
           <rPr>
@@ -1030,7 +1032,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A178" authorId="0" shapeId="0" xr:uid="{0A85963D-30AF-425D-A962-D8887D86073C}">
+    <comment ref="A178" authorId="0" shapeId="0" xr:uid="{AA017450-2F4C-4AA6-B6F4-194CC23BB6AC}">
       <text>
         <r>
           <rPr>
@@ -1054,7 +1056,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A180" authorId="0" shapeId="0" xr:uid="{3B7CCDF6-DAED-4C6F-84F5-6E00ABC604FB}">
+    <comment ref="A180" authorId="0" shapeId="0" xr:uid="{D4140002-96C2-4015-8407-CA6698F0BCCB}">
       <text>
         <r>
           <rPr>
@@ -1078,7 +1080,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A182" authorId="0" shapeId="0" xr:uid="{502F9E6F-C2E0-45CE-A8AA-B04167EC557E}">
+    <comment ref="A182" authorId="0" shapeId="0" xr:uid="{5BCBF231-D397-4D75-8A6E-EF8A716BDF09}">
       <text>
         <r>
           <rPr>
@@ -1102,7 +1104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A183" authorId="0" shapeId="0" xr:uid="{709F3016-D8B8-46D5-9AF1-357E15AEA822}">
+    <comment ref="A183" authorId="0" shapeId="0" xr:uid="{92FBB610-CE64-45E9-8CED-1551962CBF0C}">
       <text>
         <r>
           <rPr>
@@ -1126,7 +1128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A185" authorId="0" shapeId="0" xr:uid="{1BCAB7B7-E8DB-4AC9-8ABD-6F593AB9B62D}">
+    <comment ref="A185" authorId="0" shapeId="0" xr:uid="{93F5743A-67CF-4595-887D-8B704CB63E6A}">
       <text>
         <r>
           <rPr>
@@ -1150,7 +1152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A187" authorId="0" shapeId="0" xr:uid="{EBC249A3-41BE-4282-89C4-7012727505E7}">
+    <comment ref="A187" authorId="0" shapeId="0" xr:uid="{60AE20A3-3759-4BE3-9C3B-2FFA515F4531}">
       <text>
         <r>
           <rPr>
@@ -1174,7 +1176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A189" authorId="0" shapeId="0" xr:uid="{6512B587-13B7-4B2E-8923-14A44CD0F417}">
+    <comment ref="A189" authorId="0" shapeId="0" xr:uid="{71C65E76-5745-4D8B-A7C7-05EF77F31E13}">
       <text>
         <r>
           <rPr>
@@ -1198,7 +1200,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A191" authorId="0" shapeId="0" xr:uid="{C62BAA9E-6AE5-4C37-967D-045FF43C7E32}">
+    <comment ref="A191" authorId="0" shapeId="0" xr:uid="{3FD5F761-C1C2-4ABB-AB08-9E5E7DF0C401}">
       <text>
         <r>
           <rPr>
@@ -1222,7 +1224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A193" authorId="0" shapeId="0" xr:uid="{3961D8A1-2C4E-4199-9D83-5811B885AE2B}">
+    <comment ref="A193" authorId="0" shapeId="0" xr:uid="{671EAE98-0739-48FE-80DC-457B39CE2C39}">
       <text>
         <r>
           <rPr>
@@ -1246,7 +1248,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A195" authorId="0" shapeId="0" xr:uid="{37E05702-8D91-4129-847D-E292F3A432A2}">
+    <comment ref="A195" authorId="0" shapeId="0" xr:uid="{980D5BBC-A791-437E-879C-74FA51C44BF8}">
       <text>
         <r>
           <rPr>
@@ -1270,7 +1272,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A197" authorId="0" shapeId="0" xr:uid="{4A0A0C80-EE65-4962-93A7-B92C63EBCE67}">
+    <comment ref="A197" authorId="0" shapeId="0" xr:uid="{6227DA14-6BB9-4356-9AB0-C78AE1F732D1}">
       <text>
         <r>
           <rPr>
@@ -1294,7 +1296,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A199" authorId="0" shapeId="0" xr:uid="{108ED843-6BEE-4B25-8C67-DB279992F66C}">
+    <comment ref="A199" authorId="0" shapeId="0" xr:uid="{230FA2E5-500A-4F01-80F9-9C83A73F9FB8}">
       <text>
         <r>
           <rPr>
@@ -1318,7 +1320,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A201" authorId="0" shapeId="0" xr:uid="{B42E90CF-18D8-4C56-8248-DB8E9B61A9B1}">
+    <comment ref="A201" authorId="0" shapeId="0" xr:uid="{826B9C21-0026-4F9C-8483-A59B6732BA05}">
       <text>
         <r>
           <rPr>
@@ -1342,7 +1344,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A203" authorId="0" shapeId="0" xr:uid="{4025D38D-7FFF-4373-8269-1E03C515A40E}">
+    <comment ref="A203" authorId="0" shapeId="0" xr:uid="{AB52E0FA-F48F-4F9E-857D-1228386CD1A0}">
       <text>
         <r>
           <rPr>
@@ -1366,7 +1368,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A205" authorId="0" shapeId="0" xr:uid="{D38C2C85-136A-4F90-B367-B6D12465C055}">
+    <comment ref="A205" authorId="0" shapeId="0" xr:uid="{A39E2388-D488-4E53-BA41-282C8EF5A59B}">
       <text>
         <r>
           <rPr>
@@ -1390,7 +1392,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A207" authorId="0" shapeId="0" xr:uid="{03E949C1-0866-4341-9A19-E5E23B5E02D9}">
+    <comment ref="A207" authorId="0" shapeId="0" xr:uid="{C1111C54-B2C6-4FC4-BDE1-2F0248E85F5E}">
       <text>
         <r>
           <rPr>
@@ -1414,7 +1416,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A209" authorId="0" shapeId="0" xr:uid="{4DE6785A-2C72-4BDD-9C9E-F304588541DE}">
+    <comment ref="A209" authorId="0" shapeId="0" xr:uid="{85C6EEF6-AE6D-4DA9-97C3-F8A711739357}">
       <text>
         <r>
           <rPr>
@@ -1438,7 +1440,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A211" authorId="0" shapeId="0" xr:uid="{A23FD12F-17FD-4FC7-87F5-A79D6663A227}">
+    <comment ref="A211" authorId="0" shapeId="0" xr:uid="{D0CE3A08-DE92-4CBB-8B3A-9E352D406F95}">
       <text>
         <r>
           <rPr>
@@ -1462,7 +1464,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A213" authorId="0" shapeId="0" xr:uid="{75E2B4A7-C6C6-4DF6-AC61-78C637841132}">
+    <comment ref="A213" authorId="0" shapeId="0" xr:uid="{75B59AAC-0E2F-47F7-AB45-2FD5DD698626}">
       <text>
         <r>
           <rPr>
@@ -1486,7 +1488,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A215" authorId="0" shapeId="0" xr:uid="{0DED37E2-C238-46CE-BE72-DEC0E2DF18EB}">
+    <comment ref="A215" authorId="0" shapeId="0" xr:uid="{95F24AC0-CA3A-4870-BBC6-61DDD57BC25C}">
       <text>
         <r>
           <rPr>
@@ -1510,7 +1512,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A217" authorId="0" shapeId="0" xr:uid="{2111B3B9-CEBA-45D6-A08C-507D69A94B60}">
+    <comment ref="A217" authorId="0" shapeId="0" xr:uid="{00FF31DB-4969-47EB-928B-8B19B2539179}">
       <text>
         <r>
           <rPr>
@@ -1534,7 +1536,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A219" authorId="0" shapeId="0" xr:uid="{5B366D2F-155D-47A3-AF67-69648DF78F95}">
+    <comment ref="A219" authorId="0" shapeId="0" xr:uid="{7F74751B-3BCB-415F-A155-44F11FC57C7F}">
       <text>
         <r>
           <rPr>
@@ -1558,7 +1560,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A220" authorId="0" shapeId="0" xr:uid="{C6C7FDC9-E0FE-4AFE-AC89-6A4B2C6CD962}">
+    <comment ref="A220" authorId="0" shapeId="0" xr:uid="{FD609154-F141-4703-81E7-C595FC36B73B}">
       <text>
         <r>
           <rPr>
@@ -1582,7 +1584,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A222" authorId="0" shapeId="0" xr:uid="{2A024C54-9220-427D-B900-4A0D887FBAA6}">
+    <comment ref="A222" authorId="0" shapeId="0" xr:uid="{2C76003D-6DDE-40A2-AE8F-8F5F72AAC8F7}">
       <text>
         <r>
           <rPr>
@@ -1606,7 +1608,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A224" authorId="0" shapeId="0" xr:uid="{5A591208-0AAC-4268-88D7-3100A069C4EC}">
+    <comment ref="A224" authorId="0" shapeId="0" xr:uid="{76E5B7A5-602D-4AAC-AB35-F4F23416A900}">
       <text>
         <r>
           <rPr>
@@ -1630,7 +1632,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A225" authorId="0" shapeId="0" xr:uid="{7DC68AE4-3DC3-4D73-8FAC-2F70BBAF9DAA}">
+    <comment ref="A225" authorId="0" shapeId="0" xr:uid="{1949BC94-6580-4B5B-97D2-EF9CCB747FED}">
       <text>
         <r>
           <rPr>
@@ -1654,7 +1656,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A227" authorId="0" shapeId="0" xr:uid="{8E9D2C49-826A-4DA0-B49F-492ECC8F3C26}">
+    <comment ref="A227" authorId="0" shapeId="0" xr:uid="{9A6DDB06-2A8E-4A8C-A28A-E85F1470EBF8}">
       <text>
         <r>
           <rPr>
@@ -1678,7 +1680,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A229" authorId="0" shapeId="0" xr:uid="{4BEFCF1D-A56E-4EF5-9F48-5548D7026448}">
+    <comment ref="A229" authorId="0" shapeId="0" xr:uid="{302328A3-E886-47FF-AC08-B24CF2645032}">
       <text>
         <r>
           <rPr>
@@ -1702,7 +1704,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L248" authorId="0" shapeId="0" xr:uid="{F68670C7-2C99-466A-A941-0D4D6D356899}">
+    <comment ref="L248" authorId="0" shapeId="0" xr:uid="{32391C2E-CF1E-42EF-8316-89CFA9DE863C}">
       <text>
         <r>
           <rPr>
@@ -1726,7 +1728,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H252" authorId="0" shapeId="0" xr:uid="{06A5DD6B-ABAD-4DC2-BAA1-336E4A3FDF5A}">
+    <comment ref="H252" authorId="0" shapeId="0" xr:uid="{BE6E12D0-3DCD-4DEF-9F04-28F9F9C29C4B}">
       <text>
         <r>
           <rPr>
@@ -1750,7 +1752,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H257" authorId="0" shapeId="0" xr:uid="{A1DB62C9-8988-4C2D-BE10-B473779E077B}">
+    <comment ref="H257" authorId="0" shapeId="0" xr:uid="{798505ED-38A2-43D3-B7C3-BE52A71F1E60}">
       <text>
         <r>
           <rPr>
@@ -1774,7 +1776,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H275" authorId="0" shapeId="0" xr:uid="{9EE937E0-B76B-4069-A50F-E7D394DC4F6B}">
+    <comment ref="H275" authorId="0" shapeId="0" xr:uid="{363BC8BC-4B01-43FE-875C-74BBDF833CDF}">
       <text>
         <r>
           <rPr>
@@ -1798,7 +1800,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H286" authorId="0" shapeId="0" xr:uid="{9F60F576-5200-4E96-9303-BF2613E00513}">
+    <comment ref="H286" authorId="0" shapeId="0" xr:uid="{D7DCDFE0-2F1B-44B1-BE64-C3E331C781F2}">
       <text>
         <r>
           <rPr>
@@ -1822,7 +1824,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H325" authorId="0" shapeId="0" xr:uid="{589355BB-412C-4DE7-945A-7DF1EB40C4A4}">
+    <comment ref="H325" authorId="0" shapeId="0" xr:uid="{1DB3BC2E-E824-4451-A30F-2D7238937AD4}">
       <text>
         <r>
           <rPr>
@@ -1846,7 +1848,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H360" authorId="0" shapeId="0" xr:uid="{D244F96A-44CB-4828-B82F-60112DCEEC4F}">
+    <comment ref="H360" authorId="0" shapeId="0" xr:uid="{01767162-9E1C-47CF-AF81-0DEE992548D3}">
       <text>
         <r>
           <rPr>
@@ -1870,7 +1872,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K562" authorId="2" shapeId="0" xr:uid="{F20B1D46-63FF-4F8F-9E47-29C9822988CF}">
+    <comment ref="K562" authorId="2" shapeId="0" xr:uid="{4C2A750E-05A1-41F8-9C29-20796B71E5C9}">
       <text>
         <r>
           <rPr>
@@ -1899,7 +1901,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="100">
   <si>
     <t>MMXM3</t>
   </si>
@@ -2210,7 +2212,7 @@
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00000;[Red]\-&quot;R$&quot;\ #,##0.00000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2288,6 +2290,12 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -2339,7 +2347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2382,6 +2390,12 @@
     <xf numFmtId="8" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2984,7 +2998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D02C6E5-1D06-4891-85A2-FDA9A1BF5E0F}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -3696,7 +3710,382 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3D33F6-AD75-4E6F-B09E-ECEFE5FDF106}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3D33F6-AD75-4E6F-B09E-ECEFE5FDF106}">
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" style="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="41" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="41" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="41" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="41" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="41" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="41" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.7109375" style="41" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.140625" style="41" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="40"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="42"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="44">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="45">
+        <v>78174</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="44">
+        <v>39757</v>
+      </c>
+      <c r="B3" s="45">
+        <v>78174</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="44">
+        <v>39757</v>
+      </c>
+      <c r="B4" s="45">
+        <v>78174</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="43"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="44">
+        <v>39757</v>
+      </c>
+      <c r="B6" s="45">
+        <v>78174</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="44">
+        <v>39757</v>
+      </c>
+      <c r="B7" s="45">
+        <v>78174</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="44">
+        <v>39757</v>
+      </c>
+      <c r="B8" s="45">
+        <v>78174</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="43"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="44">
+        <v>39757</v>
+      </c>
+      <c r="B10" s="45">
+        <v>78174</v>
+      </c>
+      <c r="C10" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="45">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{441D5C49-7366-4947-8826-FA1DA81BF3B4}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9" t="str">
+        <f>_xlfn.CONCAT(A1,D1)</f>
+        <v>Data PregãoPapel</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C60B5A2-BB33-467C-8591-8ECD8F304B1F}">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" style="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="41" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="41" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="41" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="41" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="41" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="41" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.7109375" style="41" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.140625" style="41" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="40"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="42"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M2" s="42"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="44">
+        <v>39757</v>
+      </c>
+      <c r="B3" s="45">
+        <v>78174</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="44">
+        <v>39757</v>
+      </c>
+      <c r="B4" s="45">
+        <v>78174</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="44">
+        <v>39757</v>
+      </c>
+      <c r="B5" s="45">
+        <v>78174</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="43"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="44">
+        <v>39757</v>
+      </c>
+      <c r="B7" s="45">
+        <v>78174</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="44">
+        <v>39757</v>
+      </c>
+      <c r="B8" s="45">
+        <v>78174</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="44">
+        <v>39757</v>
+      </c>
+      <c r="B9" s="45">
+        <v>78174</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="43"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="44">
+        <v>39757</v>
+      </c>
+      <c r="B11" s="45">
+        <v>78174</v>
+      </c>
+      <c r="C11" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="45">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D567FE89-4C78-4C94-B7F2-FB3484040B1C}">
   <dimension ref="A1:AE606"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -24013,71 +24402,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{441D5C49-7366-4947-8826-FA1DA81BF3B4}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="9" t="str">
-        <f>_xlfn.CONCAT(A1,D1)</f>
-        <v>Data PregãoPapel</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22961BFF-DD8D-4DF9-844A-8A88CF7770A6}">
   <dimension ref="A1:D2"/>

</xml_diff>

<commit_message>
Filters out trailing empty lines in a 'Worksheet'.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Worksheet.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\excel\poi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FAC27D-03AA-4515-84C5-784A150605E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D73299-87C9-42B6-8FFD-303DE5B97601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" firstSheet="29" activeTab="29" xr2:uid="{2B1CA52D-E10F-49D8-8A0A-7B3A987640D9}"/>
+    <workbookView xWindow="28815" yWindow="6285" windowWidth="15750" windowHeight="12600" firstSheet="30" activeTab="31" xr2:uid="{2B1CA52D-E10F-49D8-8A0A-7B3A987640D9}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidTinyWorksheet" sheetId="25" r:id="rId1"/>
@@ -41,8 +41,10 @@
     <sheet name="BooleanInHeader" sheetId="9" r:id="rId26"/>
     <sheet name="DateInHeader" sheetId="10" r:id="rId27"/>
     <sheet name="NumericFormulaInHeader" sheetId="11" r:id="rId28"/>
-    <sheet name="GroupsNoEmptyLineAfterHeader" sheetId="3" r:id="rId29"/>
-    <sheet name="GroupsEmptyLineAfterHeader" sheetId="45" r:id="rId30"/>
+    <sheet name="TrailingEmptyLines" sheetId="46" r:id="rId29"/>
+    <sheet name="GroupsNoEmptyLineAfterHeader" sheetId="3" r:id="rId30"/>
+    <sheet name="GroupsEmptyLineAfterHeader" sheetId="45" r:id="rId31"/>
+    <sheet name="LastTwoCellsEmpty" sheetId="47" r:id="rId32"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -63,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="10">
   <si>
     <t>Data Pregão</t>
   </si>
@@ -157,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -172,6 +174,10 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1486,11 +1492,11 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3D33F6-AD75-4E6F-B09E-ECEFE5FDF106}">
-  <dimension ref="A1:M10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1849A15-E0A5-4465-9A72-50688D5EB65C}">
+  <dimension ref="A1:AB11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="A2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,7 +1519,7 @@
     <col min="16" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1528,7 +1534,7 @@
       </c>
       <c r="M1" s="10"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>39757</v>
       </c>
@@ -1542,7 +1548,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>39757</v>
       </c>
@@ -1556,7 +1562,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>39757</v>
       </c>
@@ -1570,10 +1576,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>39757</v>
       </c>
@@ -1587,7 +1593,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>39757</v>
       </c>
@@ -1601,7 +1607,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>39757</v>
       </c>
@@ -1615,10 +1621,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>39757</v>
       </c>
@@ -1632,8 +1638,30 @@
         <v>200</v>
       </c>
     </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+    <row r="11" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="17"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="16"/>
+      <c r="Z11" s="16"/>
+      <c r="AA11" s="16"/>
+      <c r="AB11" s="16"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1705,11 +1733,11 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C60B5A2-BB33-467C-8591-8ECD8F304B1F}">
-  <dimension ref="A1:M11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3D33F6-AD75-4E6F-B09E-ECEFE5FDF106}">
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1748,7 +1776,18 @@
       <c r="M1" s="10"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M2" s="10"/>
+      <c r="A2" s="12">
+        <v>39757</v>
+      </c>
+      <c r="B2" s="13">
+        <v>78174</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="13">
+        <v>200</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
@@ -1779,6 +1818,149 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>39757</v>
+      </c>
+      <c r="B6" s="13">
+        <v>78174</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>39757</v>
+      </c>
+      <c r="B7" s="13">
+        <v>78174</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>39757</v>
+      </c>
+      <c r="B8" s="13">
+        <v>78174</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>39757</v>
+      </c>
+      <c r="B10" s="13">
+        <v>78174</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="13">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C60B5A2-BB33-467C-8591-8ECD8F304B1F}">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="10"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M2" s="10"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>39757</v>
+      </c>
+      <c r="B3" s="13">
+        <v>78174</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>39757</v>
+      </c>
+      <c r="B4" s="13">
+        <v>78174</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>39757</v>
       </c>
@@ -1853,6 +2035,88 @@
       <c r="D11" s="13">
         <v>200</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{426CBC8F-7A46-4B97-AC84-7BCC1B25B3A7}">
+  <dimension ref="A1:M5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" s="10"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M2" s="10"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>39757</v>
+      </c>
+      <c r="B3" s="13">
+        <v>78174</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>39757</v>
+      </c>
+      <c r="B4" s="13">
+        <v>78174</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>39757</v>
+      </c>
+      <c r="B5" s="13">
+        <v>78174</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>